<commit_message>
(feature): autorizarHorasExtras, mapaUbicaciones y AsistenciasPorUsuario
</commit_message>
<xml_diff>
--- a/backend/testeo/Testeo control asistencias.xlsx
+++ b/backend/testeo/Testeo control asistencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elsah\OneDrive\Escritorio\Proyecto\control-asistencias\backend\testeo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A345D25D-5DED-4C25-ADE7-515E4534E93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3147EA39-0D27-494A-8E6E-C8460CB7764E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>fecha</t>
   </si>
@@ -47,9 +47,6 @@
     <t>hora salida</t>
   </si>
   <si>
-    <t>horas extras</t>
-  </si>
-  <si>
     <t>estado</t>
   </si>
   <si>
@@ -60,6 +57,15 @@
   </si>
   <si>
     <t>Sabado</t>
+  </si>
+  <si>
+    <t>horas laboradas</t>
+  </si>
+  <si>
+    <t>TARDANZA</t>
+  </si>
+  <si>
+    <t>ASISTIO</t>
   </si>
 </sst>
 </file>
@@ -379,25 +385,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P1" t="s">
         <v>2</v>
@@ -414,13 +420,13 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="N2" t="s">
         <v>4</v>
-      </c>
-      <c r="N2" t="s">
-        <v>5</v>
       </c>
       <c r="O2" s="2">
         <v>0.3125</v>
@@ -444,11 +450,14 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" s="2">
-        <f>Q2-(C3-B3)</f>
-        <v>1.3888888888888895E-2</v>
+        <f>C3-B3</f>
+        <v>0.38194444444444448</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O3" s="2">
         <v>0.3125</v>
@@ -459,6 +468,96 @@
       <c r="Q3" s="2">
         <f>P3-O3</f>
         <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45860</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="2">
+        <f>C4-B4</f>
+        <v>0.4375</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45861</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="D5" s="2">
+        <f>C5-B5</f>
+        <v>0.39166666666666666</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45862</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D6" s="2">
+        <f>C6-B6</f>
+        <v>0.39236111111111105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45863</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="2">
+        <f>C7-B7</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45773</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="D8" s="2">
+        <f>C8-B8</f>
+        <v>0.33055555555555549</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>